<commit_message>
created split plot dataset; updated all datasets; confirmed truthTableStr
created simulated split plot Excel dataset from Fed dataset: Ch00Vig5CreateSplitPlotDataset.Rmd; confirmed it is read without error.
updated datasets - see convertDatasets.R; worked on DfReadDataFile function
Discoverd that .xls input does not work; probably has to do with openxlsx;
checked truthTableStr with a data file that has only 1 and 3 lesions per case; was concerned about 4th dimension of truthTableStr; see Dropbox RJafrocChecks/truthTableStr.xlsx for results of checks; convinced it is working fine, despite my concerns; need a separate vignette on truthTableStr;
R CMD check successful; added raw excel file datasets to inst/extdata/datasets; found missing file SimulateFrocFromLrocDataset.R - not sure why I took it out
</commit_message>
<xml_diff>
--- a/inst/extdata/FrocData.xlsx
+++ b/inst/extdata/FrocData.xlsx
@@ -1,24 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6B5588-A720-8943-8333-DD256AE45B1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3611379F-CEA6-E94D-874B-0AE6B9E5AF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10700" yWindow="460" windowWidth="14860" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="660" windowWidth="14860" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TP" sheetId="3" r:id="rId1"/>
     <sheet name="FP" sheetId="2" r:id="rId2"/>
     <sheet name="Truth" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21048,7 +21056,7 @@
   <dimension ref="A1:F243"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>